<commit_message>
Fonction Login / Journeaux
Misa à jour des journeaux + Début de la fonction Login + Création des fichiers textes servant à stocker les noms d'utilisateurs et les scores
</commit_message>
<xml_diff>
--- a/Journaux_Axel.Pittet.xlsx
+++ b/Journaux_Axel.Pittet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel Pittet\Documents\GitHub\Bataille-navale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12962488-CBF9-4248-8632-59A8F1B13B65}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA28CCCB-47C4-419A-B70E-72A22B5FEEBF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>Apprentissage de comment lire et écrire sur un fichier texte extérieur au programme</t>
+  </si>
+  <si>
+    <t>https://www.developpez.net/forums/d1488547/c-cpp/c/debuter/recommencer-programme-chaine-char-oui-non/</t>
+  </si>
+  <si>
+    <t>Début du système d'authentification</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -365,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -411,6 +420,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -423,7 +435,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -432,6 +447,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -505,14 +528,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
       </border>
     </dxf>
     <dxf>
@@ -659,21 +674,21 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Projet" dataDxfId="12"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Tâche" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description / Résumé" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Sources" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Sources" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau2" displayName="Tableau2" ref="A2:E18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau2" displayName="Tableau2" ref="A2:E18" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
   <autoFilter ref="A2:E18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Qui" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Cours" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Projet" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Qui" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Cours" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Projet" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -944,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,20 +971,20 @@
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="28.44140625" customWidth="1"/>
     <col min="7" max="7" width="37.5546875" customWidth="1"/>
-    <col min="8" max="8" width="31.109375" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -993,7 +1008,7 @@
       <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="24" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1123,7 +1138,9 @@
       <c r="G7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
@@ -1147,7 +1164,9 @@
       <c r="G8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
@@ -1197,7 +1216,9 @@
       <c r="G10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
@@ -1273,7 +1294,9 @@
       <c r="G13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
@@ -1297,7 +1320,9 @@
       <c r="G14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
@@ -1321,7 +1346,9 @@
       <c r="G15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
@@ -1345,7 +1372,9 @@
       <c r="G16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
@@ -1447,19 +1476,35 @@
       <c r="G20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="4"/>
+    <row r="21" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>43925</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D21" s="9">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
@@ -2047,11 +2092,12 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H20" r:id="rId1" xr:uid="{706D1F64-60A7-4467-B9DB-E41C9154232E}"/>
+    <hyperlink ref="H21" r:id="rId2" xr:uid="{4C4507B7-83E7-462A-AB32-C03D06DCD4EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2074,13 +2120,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">

</xml_diff>